<commit_message>
Ajout nom de profil sur diagramme (#222) f4fd0954325c9b7cdce29645ebb61ee4cc4fa580
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
+++ b/main/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-03T12:52:21+00:00</t>
+    <t>2024-09-27T09:57:43+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -632,7 +632,7 @@
 * Results from operations might involve resources that are not identified.</t>
   </si>
   <si>
-    <t>fullUrl might not be [unique in the context of a resource](bundle.html#bundle-unique). Note that since [FHIR resources do not need to be served through the FHIR API](http://hl7.org/fhir/R4/references.html), the fullURL might be a URN or an absolute URL that does not end with the logical id of the resource (Resource.id). However, but if the fullUrl does look like a RESTful server URL (e.g. meets the [regex](http://hl7.org/fhir/R4/references.html#regex), then the 'id' portion of the fullUrl SHALL end with the Resource.id.
+    <t>fullUrl might not be [unique in the context of a resource](http://hl7.org/fhir/R4/bundle.html#bundle-unique). Note that since [FHIR resources do not need to be served through the FHIR API](http://hl7.org/fhir/R4/references.html), the fullURL might be a URN or an absolute URL that does not end with the logical id of the resource (Resource.id). However, but if the fullUrl does look like a RESTful server URL (e.g. meets the [regex](http://hl7.org/fhir/R4/references.html#regex), then the 'id' portion of the fullUrl SHALL end with the Resource.id.
 Note that the fullUrl is not the same as the canonical URL - it's an absolute url for an endpoint serving the resource (these will happen to have the same value on the canonical server for the resource with the canonical URL).</t>
   </si>
   <si>

</xml_diff>

<commit_message>
ANS-006-133 - Restructuration des tableaux listant les profils sur la page d'accueil et la page de ressource FHIR (#225)
* Modification de la page liste de profils et ajout d'une description à toutes les ressources

* Correction texte explicatif

* Modif index et descrfiption SDOBundle

* Correction description SD

* Modif tableau ressources et description ESMSBundle

* Update index.md

* Modification index titre

* Modification page et rnommage page liste_profil en ressource_fhir

* Fix nom page dans le yaml

* fix typo

* fix requête sql instance

* Renommage des tableaux

* Modif SQL, ajout des liens vers les ressources 459f1384407df8f502986d53e307f7f8d9461f2b
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
+++ b/main/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-02T20:14:47+00:00</t>
+    <t>2024-10-03T12:27:30+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil pour la définition du Bundle de réponse à la recherche d'une décision d'orientation ou d'une évaluation</t>
+    <t>Profil ESMS créé dans le contexte du suivi des orientations pour transporter les documents répondant à une recherche de decision ou d’évaluation.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
Sécurité - Ajouter les spécifications VT (#333)
* Update securite.md

* Update securite.md 3a0dcfd8375fd409013e4633a7e106494b890114
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
+++ b/main/ig/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-12T09:03:52+00:00</t>
+    <t>2025-06-10T12:40:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1180,17 +1180,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="21.21875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="18.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="102.5859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="87.94921875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1199,26 +1199,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="168.19140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="49.01171875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.98046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="144.1953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="28.1484375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="50.08203125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.9765625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="24.1328125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="42.9375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>